<commit_message>
Questions from James to consider
</commit_message>
<xml_diff>
--- a/timeboxes.xlsx
+++ b/timeboxes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alisha/Desktop/team-17/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asherwaqar/Desktop/team-17/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C61608D-B011-654C-B89B-AA1A8B0AE879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34EF369-0208-BC4C-9F1D-390D9FC2588A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{8E32AAB9-703C-F844-AA69-20F74C30FA84}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8E32AAB9-703C-F844-AA69-20F74C30FA84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Timebox</t>
   </si>
@@ -44,13 +44,16 @@
   <si>
     <t>Design</t>
   </si>
+  <si>
+    <t>Time Block</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -90,8 +93,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -407,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE0C50A-ECBE-DD4C-A5A1-093E1741E7E0}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -434,17 +437,17 @@
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
+      <c r="A3" s="1">
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>0.83333333333333304</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
@@ -453,119 +456,127 @@
     </row>
     <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>0.91666666666666596</v>
+        <v>0.875</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>0.95833333333333304</v>
+        <v>0.91666666666666596</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>1</v>
+        <v>0.95833333333333304</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>1.0416666666666701</v>
+        <v>1</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>1.0833333333333299</v>
+        <v>1.0416666666666701</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>1.125</v>
+        <v>1.0833333333333299</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>1.1666666666666701</v>
+        <v>1.125</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>1.2083333333333299</v>
+        <v>1.1666666666666701</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>1.25</v>
+        <v>1.2083333333333299</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>1.2916666666666701</v>
+        <v>1.25</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>1.3333333333333299</v>
+        <v>1.2916666666666701</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>1.375</v>
+        <v>1.3333333333333299</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>1.4166666666666601</v>
+        <v>1.375</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>1.4583333333333299</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>1</v>
-      </c>
+        <v>1.4166666666666601</v>
+      </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>1.5</v>
+        <v>1.4583333333333299</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>